<commit_message>
updated xsl static import to pull in measure observations
</commit_message>
<xml_diff>
--- a/test/fixtures/eh_patient_sheets/results_matrix_eh.xlsx
+++ b/test/fixtures/eh_patient_sheets/results_matrix_eh.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="46240" windowHeight="25240" tabRatio="500"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -120,13 +120,16 @@
   </si>
   <si>
     <t>RS1: ED and inpatient</t>
+  </si>
+  <si>
+    <t>OBSERV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +141,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,8 +179,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -171,7 +196,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,7 +533,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -691,14 +722,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="H12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="H12" s="4"/>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="H13" s="4"/>
@@ -744,7 +777,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G21"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -882,15 +915,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="H12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="H13" s="4"/>
@@ -949,7 +983,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G21"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1087,15 +1121,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="H12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9">
       <c r="H13" s="4"/>

</xml_diff>